<commit_message>
FIX — Lidando com valores None nas métricas. Computando métricas para resultados sem otimização.
Signed-off-by: Ariel Tadeu da Silva <silva.ariel2013@gmail.com>
</commit_message>
<xml_diff>
--- a/main/carla_runs/adult/adult_stats_carla.xlsx
+++ b/main/carla_runs/adult/adult_stats_carla.xlsx
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.5</v>
+        <v>17.75</v>
       </c>
       <c r="C3" t="n">
-        <v>1.730057634226477</v>
+        <v>12.93879281845967</v>
       </c>
       <c r="D3" t="n">
-        <v>1.667280800219122</v>
+        <v>12.7541939361204</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9518261252065576</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9045340337332909</v>
+        <v>0.4578165130223675</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9268218627522886</v>
+        <v>0.4999456601970534</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9335788775150018</v>
+        <v>0.4469435261075588</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2110529442555062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>17</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12.03676160791397</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12.00034100984755</v>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.02038468803640042</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0004155355063413665</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.02038468803640042</v>
       </c>
     </row>
     <row r="6">
@@ -538,13 +538,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C6" t="n">
-        <v>1.077501365780715</v>
+        <v>12.20948416866571</v>
       </c>
       <c r="D6" t="n">
-        <v>1.006006911156245</v>
+        <v>12.01070529872066</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -557,13 +557,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>1.144339621163123</v>
+        <v>13.18149858061092</v>
       </c>
       <c r="D7" t="n">
-        <v>1.01942369403112</v>
+        <v>13.01004228867749</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>2.284430935486671</v>
+        <v>13.25207383865541</v>
       </c>
       <c r="D8" t="n">
-        <v>2.25158065242465</v>
+        <v>13.0208299124856</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C9" t="n">
-        <v>4.056018922195868</v>
+        <v>13.5611755592543</v>
       </c>
       <c r="D9" t="n">
-        <v>4.003138119643987</v>
+        <v>13.06674066044482</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>

</xml_diff>